<commit_message>
updates for reports and MFC paper.
</commit_message>
<xml_diff>
--- a/outputs_report/Report_tables_part2(7).xlsx
+++ b/outputs_report/Report_tables_part2(7).xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F33EF0-4D59-45EB-A530-830841E7F656}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B7A7BB-0BBD-4DE8-99E8-6637C3E3DA5E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="6" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fat-tails" sheetId="10" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="175">
   <si>
     <t>Stock return</t>
   </si>
@@ -576,9 +576,6 @@
     <t>Sales tax dominant state</t>
   </si>
   <si>
-    <t>Constant growth of tax revenue</t>
-  </si>
-  <si>
     <t>returns from normal distribution</t>
   </si>
   <si>
@@ -615,21 +612,10 @@
     <t>Returns from normal distribution</t>
   </si>
   <si>
-    <t>Employer contribution as a % of payroll in year 1</t>
-  </si>
-  <si>
     <t>Probability of low funded ratio*</t>
   </si>
   <si>
     <t>Probability of sharp increase in contribution rate**</t>
-  </si>
-  <si>
-    <t>Present value of total employer contribution for 
-year 1-15***</t>
-  </si>
-  <si>
-    <t>Present value of total employer contribution for 
-year 16-30***</t>
   </si>
   <si>
     <t xml:space="preserve">Notes:
@@ -659,6 +645,35 @@
   <si>
     <t>Baseline: 
 constant growth of tax revenue</t>
+  </si>
+  <si>
+    <t>Employer contribution as a % of payroll in year 1
+(Median across 2,000 sims)</t>
+  </si>
+  <si>
+    <t>Present value of total employer contribution for 
+year 1-15***
+(Median across 2,000 sims)</t>
+  </si>
+  <si>
+    <t>Present value of total employer contribution for 
+year 16-30***
+(Median across 2,000 sims)</t>
+  </si>
+  <si>
+    <t>Assumptions about trend and cyclical growth rates of tax revenues for simulation analysis</t>
+  </si>
+  <si>
+    <t>Growth rates in inflation-adjusted tax revenue</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Individual income tax </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> General sales tax</t>
+  </si>
+  <si>
+    <t>Selective sales tax</t>
   </si>
 </sst>
 </file>
@@ -1009,7 +1024,7 @@
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="226">
+  <cellXfs count="230">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1440,55 +1455,105 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1503,30 +1568,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1548,30 +1589,54 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1581,57 +1646,19 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2728,12 +2755,12 @@
     <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
-      <c r="C3" s="160" t="s">
+      <c r="C3" s="170" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="160"/>
-      <c r="E3" s="160"/>
-      <c r="F3" s="160"/>
+      <c r="D3" s="170"/>
+      <c r="E3" s="170"/>
+      <c r="F3" s="170"/>
       <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2816,12 +2843,12 @@
     <row r="9" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="104"/>
-      <c r="C9" s="161" t="s">
+      <c r="C9" s="171" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="161"/>
-      <c r="E9" s="161"/>
-      <c r="F9" s="161"/>
+      <c r="D9" s="171"/>
+      <c r="E9" s="171"/>
+      <c r="F9" s="171"/>
       <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -2932,17 +2959,18 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3217AFE-1A01-4480-8D7E-DF20018F7399}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="21.5703125" customWidth="1"/>
-    <col min="4" max="7" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="7" width="19.7109375" customWidth="1"/>
     <col min="9" max="10" width="11" customWidth="1"/>
     <col min="11" max="11" width="10.42578125" customWidth="1"/>
     <col min="12" max="12" width="11.5703125" customWidth="1"/>
@@ -2961,119 +2989,129 @@
     <row r="2" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="98"/>
-      <c r="C2" s="161" t="s">
-        <v>144</v>
-      </c>
-      <c r="D2" s="193"/>
-      <c r="E2" s="193"/>
-      <c r="F2" s="193"/>
-      <c r="G2" s="193"/>
+      <c r="C2" s="171" t="s">
+        <v>170</v>
+      </c>
+      <c r="D2" s="203"/>
+      <c r="E2" s="203"/>
+      <c r="F2" s="203"/>
+      <c r="G2" s="203"/>
       <c r="H2" s="7"/>
     </row>
-    <row r="3" spans="1:8" s="77" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="96"/>
-      <c r="B3" s="116"/>
-      <c r="C3" s="125"/>
-      <c r="D3" s="125" t="s">
-        <v>73</v>
-      </c>
-      <c r="E3" s="125" t="s">
-        <v>74</v>
-      </c>
-      <c r="F3" s="125" t="s">
-        <v>96</v>
-      </c>
-      <c r="G3" s="125" t="s">
-        <v>75</v>
-      </c>
-      <c r="H3" s="96"/>
-    </row>
-    <row r="4" spans="1:8" s="77" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="98"/>
+      <c r="C3" s="160"/>
+      <c r="D3" s="170" t="s">
+        <v>171</v>
+      </c>
+      <c r="E3" s="170"/>
+      <c r="F3" s="170"/>
+      <c r="G3" s="170"/>
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="1:8" s="77" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="96"/>
-      <c r="B4" s="117"/>
+      <c r="B4" s="116"/>
       <c r="C4" s="125"/>
-      <c r="D4" s="169" t="s">
-        <v>94</v>
-      </c>
-      <c r="E4" s="169"/>
-      <c r="F4" s="169"/>
-      <c r="G4" s="169"/>
+      <c r="D4" s="125" t="s">
+        <v>172</v>
+      </c>
+      <c r="E4" s="125" t="s">
+        <v>173</v>
+      </c>
+      <c r="F4" s="125" t="s">
+        <v>174</v>
+      </c>
+      <c r="G4" s="125" t="s">
+        <v>61</v>
+      </c>
       <c r="H4" s="96"/>
     </row>
-    <row r="5" spans="1:8" s="77" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="77" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="96"/>
-      <c r="B5" s="169" t="s">
+      <c r="B5" s="176" t="s">
         <v>140</v>
       </c>
-      <c r="C5" s="169"/>
-      <c r="D5" s="139">
-        <v>0.02</v>
-      </c>
-      <c r="E5" s="139">
-        <v>0.02</v>
-      </c>
-      <c r="F5" s="139">
-        <v>0.02</v>
-      </c>
-      <c r="G5" s="139">
-        <v>0.02</v>
+      <c r="C5" s="176"/>
+      <c r="D5" s="229">
+        <v>1.9E-2</v>
+      </c>
+      <c r="E5" s="229">
+        <v>1.9E-2</v>
+      </c>
+      <c r="F5" s="229">
+        <v>1.9E-2</v>
+      </c>
+      <c r="G5" s="229">
+        <v>1.9E-2</v>
       </c>
       <c r="H5" s="96"/>
     </row>
-    <row r="6" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="194" t="s">
+    <row r="6" spans="1:8" s="77" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="96"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="228"/>
+      <c r="E6" s="228"/>
+      <c r="F6" s="228"/>
+      <c r="G6" s="228"/>
+      <c r="H6" s="96"/>
+    </row>
+    <row r="7" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="226" t="s">
         <v>141</v>
       </c>
-      <c r="C6" s="118" t="s">
+      <c r="C7" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="D6" s="119">
+      <c r="D7" s="161">
         <v>1</v>
       </c>
-      <c r="E6" s="119">
+      <c r="E7" s="161">
         <v>1.2</v>
       </c>
-      <c r="F6" s="120">
+      <c r="F7" s="227">
         <v>0.5</v>
       </c>
-      <c r="G6" s="119">
+      <c r="G7" s="161">
         <v>1.3</v>
       </c>
-      <c r="H6" s="7"/>
-    </row>
-    <row r="7" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="190"/>
-      <c r="C7" s="124" t="s">
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="200"/>
+      <c r="C8" s="124" t="s">
         <v>142</v>
       </c>
-      <c r="D7" s="128">
+      <c r="D8" s="128">
         <v>0.2</v>
       </c>
-      <c r="E7" s="128" t="s">
+      <c r="E8" s="128" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="128" t="s">
+      <c r="F8" s="128" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="128" t="s">
+      <c r="G8" s="128" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="7"/>
-    </row>
-    <row r="8" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="H8" s="7"/>
+    </row>
     <row r="9" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="C2:G2"/>
-    <mergeCell ref="D4:G4"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="D3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3105,13 +3143,13 @@
     </row>
     <row r="2" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27"/>
-      <c r="B2" s="161" t="s">
+      <c r="B2" s="171" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="161"/>
-      <c r="D2" s="161"/>
-      <c r="E2" s="161"/>
-      <c r="F2" s="161"/>
+      <c r="C2" s="171"/>
+      <c r="D2" s="171"/>
+      <c r="E2" s="171"/>
+      <c r="F2" s="171"/>
       <c r="G2" s="27"/>
       <c r="H2" s="27"/>
     </row>
@@ -3236,7 +3274,7 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="G16" sqref="G16:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3251,23 +3289,23 @@
   <sheetData>
     <row r="1" spans="2:14" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:14" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="196" t="s">
-        <v>166</v>
-      </c>
-      <c r="C2" s="197"/>
-      <c r="D2" s="197"/>
-      <c r="E2" s="197"/>
-      <c r="F2" s="197"/>
-      <c r="G2" s="197"/>
-      <c r="H2" s="197"/>
+      <c r="B2" s="213" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" s="214"/>
+      <c r="D2" s="214"/>
+      <c r="E2" s="214"/>
+      <c r="F2" s="214"/>
+      <c r="G2" s="214"/>
+      <c r="H2" s="214"/>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
     </row>
     <row r="3" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="140"/>
       <c r="C3" s="141"/>
-      <c r="D3" s="213" t="s">
-        <v>167</v>
+      <c r="D3" s="207" t="s">
+        <v>163</v>
       </c>
       <c r="E3" s="152" t="s">
         <v>145</v>
@@ -3275,36 +3313,36 @@
       <c r="F3" s="152" t="s">
         <v>146</v>
       </c>
-      <c r="G3" s="213" t="s">
-        <v>170</v>
-      </c>
-      <c r="H3" s="225"/>
+      <c r="G3" s="207" t="s">
+        <v>166</v>
+      </c>
+      <c r="H3" s="208"/>
     </row>
     <row r="4" spans="2:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="218"/>
-      <c r="C4" s="216"/>
+      <c r="B4" s="166"/>
+      <c r="C4" s="164"/>
       <c r="D4" s="212"/>
       <c r="E4" s="143" t="s">
+        <v>155</v>
+      </c>
+      <c r="F4" s="143" t="s">
         <v>156</v>
       </c>
-      <c r="F4" s="143" t="s">
+      <c r="G4" s="143" t="s">
+        <v>155</v>
+      </c>
+      <c r="H4" s="144" t="s">
         <v>157</v>
       </c>
-      <c r="G4" s="143" t="s">
-        <v>156</v>
-      </c>
-      <c r="H4" s="144" t="s">
-        <v>158</v>
-      </c>
     </row>
     <row r="5" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="219" t="s">
-        <v>168</v>
-      </c>
-      <c r="C5" s="220" t="s">
-        <v>152</v>
-      </c>
-      <c r="D5" s="214">
+      <c r="B5" s="209" t="s">
+        <v>164</v>
+      </c>
+      <c r="C5" s="167" t="s">
+        <v>151</v>
+      </c>
+      <c r="D5" s="162">
         <v>7.2400000000000006E-2</v>
       </c>
       <c r="E5" s="145">
@@ -3337,11 +3375,11 @@
       </c>
     </row>
     <row r="6" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="221"/>
-      <c r="C6" s="220" t="s">
-        <v>153</v>
-      </c>
-      <c r="D6" s="215">
+      <c r="B6" s="210"/>
+      <c r="C6" s="167" t="s">
+        <v>152</v>
+      </c>
+      <c r="D6" s="163">
         <v>0.05</v>
       </c>
       <c r="E6" s="145">
@@ -3374,9 +3412,9 @@
       </c>
     </row>
     <row r="7" spans="2:14" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="222"/>
-      <c r="C7" s="220"/>
-      <c r="D7" s="216"/>
+      <c r="B7" s="168"/>
+      <c r="C7" s="167"/>
+      <c r="D7" s="164"/>
       <c r="E7" s="145"/>
       <c r="F7" s="145"/>
       <c r="G7" s="145"/>
@@ -3395,13 +3433,13 @@
       </c>
     </row>
     <row r="8" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="219" t="s">
-        <v>169</v>
-      </c>
-      <c r="C8" s="220" t="s">
-        <v>152</v>
-      </c>
-      <c r="D8" s="214">
+      <c r="B8" s="209" t="s">
+        <v>165</v>
+      </c>
+      <c r="C8" s="167" t="s">
+        <v>151</v>
+      </c>
+      <c r="D8" s="162">
         <v>0.12720000000000001</v>
       </c>
       <c r="E8" s="145">
@@ -3434,11 +3472,11 @@
       </c>
     </row>
     <row r="9" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="223"/>
-      <c r="C9" s="224" t="s">
-        <v>153</v>
-      </c>
-      <c r="D9" s="217">
+      <c r="B9" s="211"/>
+      <c r="C9" s="169" t="s">
+        <v>152</v>
+      </c>
+      <c r="D9" s="165">
         <v>8.48E-2</v>
       </c>
       <c r="E9" s="149">
@@ -3459,15 +3497,15 @@
       </c>
     </row>
     <row r="10" spans="2:14" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="202" t="s">
-        <v>154</v>
-      </c>
-      <c r="C10" s="202"/>
-      <c r="D10" s="202"/>
-      <c r="E10" s="202"/>
-      <c r="F10" s="202"/>
-      <c r="G10" s="202"/>
-      <c r="H10" s="202"/>
+      <c r="B10" s="206" t="s">
+        <v>153</v>
+      </c>
+      <c r="C10" s="206"/>
+      <c r="D10" s="206"/>
+      <c r="E10" s="206"/>
+      <c r="F10" s="206"/>
+      <c r="G10" s="206"/>
+      <c r="H10" s="206"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
@@ -3482,21 +3520,21 @@
     <row r="13" spans="2:14" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="2:14" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="2:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="196" t="s">
-        <v>165</v>
-      </c>
-      <c r="C15" s="197"/>
-      <c r="D15" s="197"/>
-      <c r="E15" s="197"/>
-      <c r="F15" s="197"/>
-      <c r="G15" s="197"/>
-      <c r="H15" s="197"/>
+      <c r="B15" s="213" t="s">
+        <v>161</v>
+      </c>
+      <c r="C15" s="214"/>
+      <c r="D15" s="214"/>
+      <c r="E15" s="214"/>
+      <c r="F15" s="214"/>
+      <c r="G15" s="214"/>
+      <c r="H15" s="214"/>
     </row>
     <row r="16" spans="2:14" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="140"/>
       <c r="C16" s="141"/>
-      <c r="D16" s="213" t="s">
-        <v>167</v>
+      <c r="D16" s="207" t="s">
+        <v>163</v>
       </c>
       <c r="E16" s="152" t="s">
         <v>145</v>
@@ -3504,36 +3542,36 @@
       <c r="F16" s="152" t="s">
         <v>146</v>
       </c>
-      <c r="G16" s="213" t="s">
-        <v>170</v>
-      </c>
-      <c r="H16" s="225"/>
+      <c r="G16" s="207" t="s">
+        <v>166</v>
+      </c>
+      <c r="H16" s="208"/>
     </row>
     <row r="17" spans="2:14" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="142"/>
       <c r="C17" s="93"/>
       <c r="D17" s="212"/>
       <c r="E17" s="143" t="s">
+        <v>155</v>
+      </c>
+      <c r="F17" s="143" t="s">
         <v>156</v>
       </c>
-      <c r="F17" s="143" t="s">
+      <c r="G17" s="143" t="s">
+        <v>155</v>
+      </c>
+      <c r="H17" s="144" t="s">
         <v>157</v>
       </c>
-      <c r="G17" s="143" t="s">
-        <v>156</v>
-      </c>
-      <c r="H17" s="144" t="s">
-        <v>158</v>
-      </c>
     </row>
     <row r="18" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="219" t="s">
-        <v>168</v>
-      </c>
-      <c r="C18" s="220" t="s">
-        <v>152</v>
-      </c>
-      <c r="D18" s="214">
+      <c r="B18" s="209" t="s">
+        <v>164</v>
+      </c>
+      <c r="C18" s="167" t="s">
+        <v>151</v>
+      </c>
+      <c r="D18" s="162">
         <v>7.2400000000000006E-2</v>
       </c>
       <c r="E18" s="145">
@@ -3566,11 +3604,11 @@
       </c>
     </row>
     <row r="19" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="221"/>
-      <c r="C19" s="220" t="s">
-        <v>153</v>
-      </c>
-      <c r="D19" s="215">
+      <c r="B19" s="210"/>
+      <c r="C19" s="167" t="s">
+        <v>152</v>
+      </c>
+      <c r="D19" s="163">
         <v>0.05</v>
       </c>
       <c r="E19" s="145">
@@ -3603,9 +3641,9 @@
       </c>
     </row>
     <row r="20" spans="2:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="222"/>
-      <c r="C20" s="220"/>
-      <c r="D20" s="216"/>
+      <c r="B20" s="168"/>
+      <c r="C20" s="167"/>
+      <c r="D20" s="164"/>
       <c r="E20" s="145"/>
       <c r="F20" s="145"/>
       <c r="G20" s="145"/>
@@ -3624,13 +3662,13 @@
       </c>
     </row>
     <row r="21" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="219" t="s">
-        <v>169</v>
-      </c>
-      <c r="C21" s="220" t="s">
-        <v>152</v>
-      </c>
-      <c r="D21" s="214">
+      <c r="B21" s="209" t="s">
+        <v>165</v>
+      </c>
+      <c r="C21" s="167" t="s">
+        <v>151</v>
+      </c>
+      <c r="D21" s="162">
         <v>0.12720000000000001</v>
       </c>
       <c r="E21" s="145">
@@ -3663,11 +3701,11 @@
       </c>
     </row>
     <row r="22" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="223"/>
-      <c r="C22" s="224" t="s">
-        <v>153</v>
-      </c>
-      <c r="D22" s="217">
+      <c r="B22" s="211"/>
+      <c r="C22" s="169" t="s">
+        <v>152</v>
+      </c>
+      <c r="D22" s="165">
         <v>8.48E-2</v>
       </c>
       <c r="E22" s="149">
@@ -3688,15 +3726,15 @@
       </c>
     </row>
     <row r="23" spans="2:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="202" t="s">
-        <v>154</v>
-      </c>
-      <c r="C23" s="202"/>
-      <c r="D23" s="202"/>
-      <c r="E23" s="202"/>
-      <c r="F23" s="202"/>
-      <c r="G23" s="202"/>
-      <c r="H23" s="202"/>
+      <c r="B23" s="206" t="s">
+        <v>153</v>
+      </c>
+      <c r="C23" s="206"/>
+      <c r="D23" s="206"/>
+      <c r="E23" s="206"/>
+      <c r="F23" s="206"/>
+      <c r="G23" s="206"/>
+      <c r="H23" s="206"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" s="7"/>
@@ -3796,6 +3834,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B21:B22"/>
     <mergeCell ref="B23:H23"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="B5:B6"/>
@@ -3803,11 +3846,6 @@
     <mergeCell ref="B10:H10"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="D16:D17"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B21:B22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3817,8 +3855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD5020AD-1954-4ED3-85EA-DC4DA14EE02C}">
   <dimension ref="A2:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3830,14 +3868,14 @@
   <sheetData>
     <row r="2" spans="1:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
-      <c r="B2" s="196" t="s">
-        <v>155</v>
-      </c>
-      <c r="C2" s="197"/>
-      <c r="D2" s="197"/>
-      <c r="E2" s="197"/>
-      <c r="F2" s="197"/>
-      <c r="G2" s="197"/>
+      <c r="B2" s="213" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2" s="214"/>
+      <c r="D2" s="214"/>
+      <c r="E2" s="214"/>
+      <c r="F2" s="214"/>
+      <c r="G2" s="214"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
@@ -3852,10 +3890,10 @@
       <c r="E3" s="152" t="s">
         <v>146</v>
       </c>
-      <c r="F3" s="198" t="s">
-        <v>147</v>
-      </c>
-      <c r="G3" s="199"/>
+      <c r="F3" s="207" t="s">
+        <v>166</v>
+      </c>
+      <c r="G3" s="208"/>
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3863,26 +3901,26 @@
       <c r="B4" s="142"/>
       <c r="C4" s="93"/>
       <c r="D4" s="143" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E4" s="143" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F4" s="143" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G4" s="144" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
-      <c r="B5" s="200" t="s">
-        <v>150</v>
+      <c r="B5" s="215" t="s">
+        <v>149</v>
       </c>
       <c r="C5" s="93" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D5" s="145">
         <f>J5</f>
@@ -3916,9 +3954,9 @@
     </row>
     <row r="6" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
-      <c r="B6" s="200"/>
+      <c r="B6" s="215"/>
       <c r="C6" s="93" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D6" s="145">
         <f>J6</f>
@@ -3974,11 +4012,11 @@
     </row>
     <row r="8" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
-      <c r="B8" s="200" t="s">
+      <c r="B8" s="215" t="s">
+        <v>150</v>
+      </c>
+      <c r="C8" s="93" t="s">
         <v>151</v>
-      </c>
-      <c r="C8" s="93" t="s">
-        <v>152</v>
       </c>
       <c r="D8" s="145">
         <f>J7</f>
@@ -4012,9 +4050,9 @@
     </row>
     <row r="9" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
-      <c r="B9" s="201"/>
+      <c r="B9" s="216"/>
       <c r="C9" s="148" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D9" s="149">
         <f>J8</f>
@@ -4036,14 +4074,14 @@
     </row>
     <row r="10" spans="1:13" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
-      <c r="B10" s="202" t="s">
-        <v>154</v>
-      </c>
-      <c r="C10" s="202"/>
-      <c r="D10" s="202"/>
-      <c r="E10" s="202"/>
-      <c r="F10" s="202"/>
-      <c r="G10" s="202"/>
+      <c r="B10" s="206" t="s">
+        <v>153</v>
+      </c>
+      <c r="C10" s="206"/>
+      <c r="D10" s="206"/>
+      <c r="E10" s="206"/>
+      <c r="F10" s="206"/>
+      <c r="G10" s="206"/>
       <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -4154,7 +4192,7 @@
   <dimension ref="A2:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4178,31 +4216,31 @@
       <c r="G2" s="98"/>
       <c r="H2" s="98"/>
     </row>
-    <row r="3" spans="2:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="158"/>
       <c r="C3" s="159"/>
       <c r="D3" s="127" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E3" s="127" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F3" s="127" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="G3" s="127" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="H3" s="127" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="170" t="s">
-        <v>150</v>
+      <c r="B4" s="179" t="s">
+        <v>149</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D4" s="78">
         <v>7.2463768115942032E-2</v>
@@ -4229,9 +4267,9 @@
       </c>
     </row>
     <row r="5" spans="2:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="170"/>
+      <c r="B5" s="179"/>
       <c r="C5" s="24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D5" s="78">
         <v>0.32433783108445779</v>
@@ -4267,11 +4305,11 @@
       <c r="H6" s="43"/>
     </row>
     <row r="7" spans="2:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="170" t="s">
+      <c r="B7" s="179" t="s">
+        <v>150</v>
+      </c>
+      <c r="C7" s="24" t="s">
         <v>151</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>152</v>
       </c>
       <c r="D7" s="78">
         <v>6.9965017491254375E-3</v>
@@ -4298,9 +4336,9 @@
       </c>
     </row>
     <row r="8" spans="2:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="193"/>
+      <c r="B8" s="203"/>
       <c r="C8" s="124" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D8" s="80">
         <v>0.10444777611194402</v>
@@ -4327,15 +4365,15 @@
       </c>
     </row>
     <row r="9" spans="2:11" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="187" t="s">
-        <v>164</v>
-      </c>
-      <c r="C9" s="187"/>
-      <c r="D9" s="187"/>
-      <c r="E9" s="187"/>
-      <c r="F9" s="187"/>
-      <c r="G9" s="187"/>
-      <c r="H9" s="187"/>
+      <c r="B9" s="189" t="s">
+        <v>160</v>
+      </c>
+      <c r="C9" s="189"/>
+      <c r="D9" s="189"/>
+      <c r="E9" s="189"/>
+      <c r="F9" s="189"/>
+      <c r="G9" s="189"/>
+      <c r="H9" s="189"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4379,71 +4417,71 @@
     </row>
     <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27"/>
-      <c r="B2" s="162" t="s">
+      <c r="B2" s="185" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
-      <c r="I2" s="163"/>
-      <c r="J2" s="163"/>
-      <c r="K2" s="163"/>
-      <c r="L2" s="163"/>
+      <c r="C2" s="186"/>
+      <c r="D2" s="186"/>
+      <c r="E2" s="186"/>
+      <c r="F2" s="186"/>
+      <c r="G2" s="186"/>
+      <c r="H2" s="186"/>
+      <c r="I2" s="186"/>
+      <c r="J2" s="186"/>
+      <c r="K2" s="186"/>
+      <c r="L2" s="186"/>
       <c r="M2" s="27"/>
       <c r="N2" s="7"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="27"/>
       <c r="B3" s="30"/>
-      <c r="C3" s="164" t="s">
+      <c r="C3" s="182" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="165"/>
-      <c r="E3" s="164" t="s">
+      <c r="D3" s="183"/>
+      <c r="E3" s="182" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="165"/>
-      <c r="G3" s="164" t="s">
+      <c r="F3" s="183"/>
+      <c r="G3" s="182" t="s">
         <v>38</v>
       </c>
-      <c r="H3" s="165"/>
-      <c r="I3" s="164" t="s">
+      <c r="H3" s="183"/>
+      <c r="I3" s="182" t="s">
         <v>39</v>
       </c>
-      <c r="J3" s="165"/>
-      <c r="K3" s="164" t="s">
+      <c r="J3" s="183"/>
+      <c r="K3" s="182" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="165"/>
+      <c r="L3" s="183"/>
       <c r="M3" s="27"/>
       <c r="N3" s="7"/>
     </row>
     <row r="4" spans="1:14" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="27"/>
       <c r="B4" s="30"/>
-      <c r="C4" s="160" t="s">
+      <c r="C4" s="170" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="165"/>
-      <c r="E4" s="167" t="s">
+      <c r="D4" s="183"/>
+      <c r="E4" s="178" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="168"/>
-      <c r="G4" s="169" t="s">
+      <c r="F4" s="177"/>
+      <c r="G4" s="176" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="168"/>
-      <c r="I4" s="167" t="s">
+      <c r="H4" s="177"/>
+      <c r="I4" s="178" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="168"/>
-      <c r="K4" s="169" t="s">
+      <c r="J4" s="177"/>
+      <c r="K4" s="176" t="s">
         <v>35</v>
       </c>
-      <c r="L4" s="169"/>
+      <c r="L4" s="176"/>
       <c r="M4" s="27"/>
       <c r="N4" s="7"/>
     </row>
@@ -4734,26 +4772,26 @@
       <c r="B16" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="170">
+      <c r="C16" s="179">
         <v>38</v>
       </c>
-      <c r="D16" s="171"/>
-      <c r="E16" s="172">
+      <c r="D16" s="180"/>
+      <c r="E16" s="181">
         <v>38</v>
       </c>
-      <c r="F16" s="171"/>
-      <c r="G16" s="170">
+      <c r="F16" s="180"/>
+      <c r="G16" s="179">
         <v>38</v>
       </c>
-      <c r="H16" s="171"/>
-      <c r="I16" s="172">
+      <c r="H16" s="180"/>
+      <c r="I16" s="181">
         <v>38</v>
       </c>
-      <c r="J16" s="171"/>
-      <c r="K16" s="170">
+      <c r="J16" s="180"/>
+      <c r="K16" s="179">
         <v>38</v>
       </c>
-      <c r="L16" s="170"/>
+      <c r="L16" s="179"/>
       <c r="M16" s="27"/>
       <c r="N16" s="7"/>
     </row>
@@ -4787,19 +4825,19 @@
     </row>
     <row r="18" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="27"/>
-      <c r="B18" s="162" t="s">
+      <c r="B18" s="185" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="163"/>
-      <c r="D18" s="163"/>
-      <c r="E18" s="163"/>
-      <c r="F18" s="163"/>
-      <c r="G18" s="163"/>
-      <c r="H18" s="163"/>
-      <c r="I18" s="163"/>
-      <c r="J18" s="163"/>
-      <c r="K18" s="163"/>
-      <c r="L18" s="163"/>
+      <c r="C18" s="186"/>
+      <c r="D18" s="186"/>
+      <c r="E18" s="186"/>
+      <c r="F18" s="186"/>
+      <c r="G18" s="186"/>
+      <c r="H18" s="186"/>
+      <c r="I18" s="186"/>
+      <c r="J18" s="186"/>
+      <c r="K18" s="186"/>
+      <c r="L18" s="186"/>
       <c r="M18" s="27"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -4809,18 +4847,18 @@
       <c r="D19" s="24"/>
       <c r="E19" s="17"/>
       <c r="F19" s="52"/>
-      <c r="G19" s="164" t="s">
+      <c r="G19" s="182" t="s">
         <v>41</v>
       </c>
-      <c r="H19" s="165"/>
-      <c r="I19" s="164" t="s">
+      <c r="H19" s="183"/>
+      <c r="I19" s="182" t="s">
         <v>42</v>
       </c>
-      <c r="J19" s="165"/>
-      <c r="K19" s="164" t="s">
+      <c r="J19" s="183"/>
+      <c r="K19" s="182" t="s">
         <v>43</v>
       </c>
-      <c r="L19" s="165"/>
+      <c r="L19" s="183"/>
       <c r="M19" s="27"/>
     </row>
     <row r="20" spans="1:14" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4830,18 +4868,18 @@
       <c r="D20" s="24"/>
       <c r="E20" s="17"/>
       <c r="F20" s="52"/>
-      <c r="G20" s="176" t="s">
+      <c r="G20" s="184" t="s">
         <v>5</v>
       </c>
-      <c r="H20" s="165"/>
-      <c r="I20" s="167" t="s">
+      <c r="H20" s="183"/>
+      <c r="I20" s="178" t="s">
         <v>25</v>
       </c>
-      <c r="J20" s="168"/>
-      <c r="K20" s="169" t="s">
+      <c r="J20" s="177"/>
+      <c r="K20" s="176" t="s">
         <v>26</v>
       </c>
-      <c r="L20" s="169"/>
+      <c r="L20" s="176"/>
       <c r="M20" s="27"/>
     </row>
     <row r="21" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.25">
@@ -5088,18 +5126,18 @@
       <c r="D32" s="20"/>
       <c r="E32" s="20"/>
       <c r="F32" s="54"/>
-      <c r="G32" s="172">
+      <c r="G32" s="181">
         <v>38</v>
       </c>
-      <c r="H32" s="171"/>
-      <c r="I32" s="172">
+      <c r="H32" s="180"/>
+      <c r="I32" s="181">
         <v>38</v>
       </c>
-      <c r="J32" s="171"/>
-      <c r="K32" s="170">
+      <c r="J32" s="180"/>
+      <c r="K32" s="179">
         <v>38</v>
       </c>
-      <c r="L32" s="170"/>
+      <c r="L32" s="179"/>
       <c r="M32" s="27"/>
     </row>
     <row r="33" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5213,12 +5251,12 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B45" s="24"/>
-      <c r="G45" s="169"/>
-      <c r="H45" s="168"/>
-      <c r="I45" s="167"/>
-      <c r="J45" s="168"/>
-      <c r="K45" s="169"/>
-      <c r="L45" s="169"/>
+      <c r="G45" s="176"/>
+      <c r="H45" s="177"/>
+      <c r="I45" s="178"/>
+      <c r="J45" s="177"/>
+      <c r="K45" s="176"/>
+      <c r="L45" s="176"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B46" s="24"/>
@@ -5317,12 +5355,12 @@
       <c r="L56" s="19"/>
     </row>
     <row r="57" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="G57" s="170"/>
-      <c r="H57" s="171"/>
-      <c r="I57" s="172"/>
-      <c r="J57" s="171"/>
-      <c r="K57" s="170"/>
-      <c r="L57" s="170"/>
+      <c r="G57" s="179"/>
+      <c r="H57" s="180"/>
+      <c r="I57" s="181"/>
+      <c r="J57" s="180"/>
+      <c r="K57" s="179"/>
+      <c r="L57" s="179"/>
     </row>
     <row r="58" spans="2:12" x14ac:dyDescent="0.25">
       <c r="G58" s="173"/>
@@ -5334,27 +5372,12 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="I58:J58"/>
-    <mergeCell ref="K58:L58"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="K45:L45"/>
-    <mergeCell ref="G57:H57"/>
-    <mergeCell ref="I57:J57"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
     <mergeCell ref="B18:L18"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="E4:F4"/>
@@ -5371,12 +5394,27 @@
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="I17:J17"/>
     <mergeCell ref="K17:L17"/>
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="K58:L58"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="K45:L45"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="K57:L57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -5403,14 +5441,14 @@
   <sheetData>
     <row r="2" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
-      <c r="B2" s="203" t="s">
+      <c r="B2" s="217" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="203"/>
-      <c r="D2" s="203"/>
-      <c r="E2" s="203"/>
-      <c r="F2" s="203"/>
-      <c r="G2" s="203"/>
+      <c r="C2" s="217"/>
+      <c r="D2" s="217"/>
+      <c r="E2" s="217"/>
+      <c r="F2" s="217"/>
+      <c r="G2" s="217"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
     </row>
@@ -5678,14 +5716,14 @@
       <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="203" t="s">
+      <c r="B16" s="217" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="203"/>
-      <c r="D16" s="203"/>
-      <c r="E16" s="203"/>
-      <c r="F16" s="203"/>
-      <c r="G16" s="203"/>
+      <c r="C16" s="217"/>
+      <c r="D16" s="217"/>
+      <c r="E16" s="217"/>
+      <c r="F16" s="217"/>
+      <c r="G16" s="217"/>
     </row>
     <row r="17" spans="2:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="8"/>
@@ -5913,71 +5951,71 @@
     </row>
     <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27"/>
-      <c r="B2" s="162" t="s">
+      <c r="B2" s="185" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
-      <c r="I2" s="163"/>
-      <c r="J2" s="163"/>
-      <c r="K2" s="163"/>
-      <c r="L2" s="163"/>
+      <c r="C2" s="186"/>
+      <c r="D2" s="186"/>
+      <c r="E2" s="186"/>
+      <c r="F2" s="186"/>
+      <c r="G2" s="186"/>
+      <c r="H2" s="186"/>
+      <c r="I2" s="186"/>
+      <c r="J2" s="186"/>
+      <c r="K2" s="186"/>
+      <c r="L2" s="186"/>
       <c r="M2" s="27"/>
       <c r="N2" s="7"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="27"/>
       <c r="B3" s="30"/>
-      <c r="C3" s="164" t="s">
+      <c r="C3" s="182" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="165"/>
-      <c r="E3" s="164" t="s">
+      <c r="D3" s="183"/>
+      <c r="E3" s="182" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="165"/>
-      <c r="G3" s="164" t="s">
+      <c r="F3" s="183"/>
+      <c r="G3" s="182" t="s">
         <v>38</v>
       </c>
-      <c r="H3" s="165"/>
-      <c r="I3" s="164" t="s">
+      <c r="H3" s="183"/>
+      <c r="I3" s="182" t="s">
         <v>39</v>
       </c>
-      <c r="J3" s="165"/>
-      <c r="K3" s="164" t="s">
+      <c r="J3" s="183"/>
+      <c r="K3" s="182" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="165"/>
+      <c r="L3" s="183"/>
       <c r="M3" s="27"/>
       <c r="N3" s="7"/>
     </row>
     <row r="4" spans="1:14" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="27"/>
       <c r="B4" s="30"/>
-      <c r="C4" s="160" t="s">
+      <c r="C4" s="170" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="165"/>
-      <c r="E4" s="167" t="s">
+      <c r="D4" s="183"/>
+      <c r="E4" s="178" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="168"/>
-      <c r="G4" s="169" t="s">
+      <c r="F4" s="177"/>
+      <c r="G4" s="176" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="168"/>
-      <c r="I4" s="167" t="s">
+      <c r="H4" s="177"/>
+      <c r="I4" s="178" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="168"/>
-      <c r="K4" s="169" t="s">
+      <c r="J4" s="177"/>
+      <c r="K4" s="176" t="s">
         <v>35</v>
       </c>
-      <c r="L4" s="169"/>
+      <c r="L4" s="176"/>
       <c r="M4" s="27"/>
       <c r="N4" s="7"/>
     </row>
@@ -6268,26 +6306,26 @@
       <c r="B16" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="170">
+      <c r="C16" s="179">
         <v>38</v>
       </c>
-      <c r="D16" s="171"/>
-      <c r="E16" s="172">
+      <c r="D16" s="180"/>
+      <c r="E16" s="181">
         <v>38</v>
       </c>
-      <c r="F16" s="171"/>
-      <c r="G16" s="170">
+      <c r="F16" s="180"/>
+      <c r="G16" s="179">
         <v>38</v>
       </c>
-      <c r="H16" s="171"/>
-      <c r="I16" s="172">
+      <c r="H16" s="180"/>
+      <c r="I16" s="181">
         <v>38</v>
       </c>
-      <c r="J16" s="171"/>
-      <c r="K16" s="170">
+      <c r="J16" s="180"/>
+      <c r="K16" s="179">
         <v>38</v>
       </c>
-      <c r="L16" s="170"/>
+      <c r="L16" s="179"/>
       <c r="M16" s="27"/>
       <c r="N16" s="7"/>
     </row>
@@ -6321,19 +6359,19 @@
     </row>
     <row r="18" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="27"/>
-      <c r="B18" s="162" t="s">
+      <c r="B18" s="185" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="163"/>
-      <c r="D18" s="163"/>
-      <c r="E18" s="163"/>
-      <c r="F18" s="163"/>
-      <c r="G18" s="163"/>
-      <c r="H18" s="163"/>
-      <c r="I18" s="163"/>
-      <c r="J18" s="163"/>
-      <c r="K18" s="163"/>
-      <c r="L18" s="163"/>
+      <c r="C18" s="186"/>
+      <c r="D18" s="186"/>
+      <c r="E18" s="186"/>
+      <c r="F18" s="186"/>
+      <c r="G18" s="186"/>
+      <c r="H18" s="186"/>
+      <c r="I18" s="186"/>
+      <c r="J18" s="186"/>
+      <c r="K18" s="186"/>
+      <c r="L18" s="186"/>
       <c r="M18" s="27"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -6343,18 +6381,18 @@
       <c r="D19" s="24"/>
       <c r="E19" s="17"/>
       <c r="F19" s="52"/>
-      <c r="G19" s="164" t="s">
+      <c r="G19" s="182" t="s">
         <v>41</v>
       </c>
-      <c r="H19" s="165"/>
-      <c r="I19" s="164" t="s">
+      <c r="H19" s="183"/>
+      <c r="I19" s="182" t="s">
         <v>42</v>
       </c>
-      <c r="J19" s="165"/>
-      <c r="K19" s="164" t="s">
+      <c r="J19" s="183"/>
+      <c r="K19" s="182" t="s">
         <v>43</v>
       </c>
-      <c r="L19" s="165"/>
+      <c r="L19" s="183"/>
       <c r="M19" s="27"/>
     </row>
     <row r="20" spans="1:14" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6364,18 +6402,18 @@
       <c r="D20" s="24"/>
       <c r="E20" s="17"/>
       <c r="F20" s="52"/>
-      <c r="G20" s="176" t="s">
+      <c r="G20" s="184" t="s">
         <v>5</v>
       </c>
-      <c r="H20" s="165"/>
-      <c r="I20" s="167" t="s">
+      <c r="H20" s="183"/>
+      <c r="I20" s="178" t="s">
         <v>25</v>
       </c>
-      <c r="J20" s="168"/>
-      <c r="K20" s="169" t="s">
+      <c r="J20" s="177"/>
+      <c r="K20" s="176" t="s">
         <v>26</v>
       </c>
-      <c r="L20" s="169"/>
+      <c r="L20" s="176"/>
       <c r="M20" s="27"/>
     </row>
     <row r="21" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.25">
@@ -6622,18 +6660,18 @@
       <c r="D32" s="20"/>
       <c r="E32" s="20"/>
       <c r="F32" s="54"/>
-      <c r="G32" s="172">
+      <c r="G32" s="181">
         <v>38</v>
       </c>
-      <c r="H32" s="171"/>
-      <c r="I32" s="172">
+      <c r="H32" s="180"/>
+      <c r="I32" s="181">
         <v>38</v>
       </c>
-      <c r="J32" s="171"/>
-      <c r="K32" s="170">
+      <c r="J32" s="180"/>
+      <c r="K32" s="179">
         <v>38</v>
       </c>
-      <c r="L32" s="170"/>
+      <c r="L32" s="179"/>
       <c r="M32" s="27"/>
     </row>
     <row r="33" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6747,12 +6785,12 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B45" s="24"/>
-      <c r="G45" s="169"/>
-      <c r="H45" s="168"/>
-      <c r="I45" s="167"/>
-      <c r="J45" s="168"/>
-      <c r="K45" s="169"/>
-      <c r="L45" s="169"/>
+      <c r="G45" s="176"/>
+      <c r="H45" s="177"/>
+      <c r="I45" s="178"/>
+      <c r="J45" s="177"/>
+      <c r="K45" s="176"/>
+      <c r="L45" s="176"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B46" s="24"/>
@@ -6851,12 +6889,12 @@
       <c r="L56" s="19"/>
     </row>
     <row r="57" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="G57" s="170"/>
-      <c r="H57" s="171"/>
-      <c r="I57" s="172"/>
-      <c r="J57" s="171"/>
-      <c r="K57" s="170"/>
-      <c r="L57" s="170"/>
+      <c r="G57" s="179"/>
+      <c r="H57" s="180"/>
+      <c r="I57" s="181"/>
+      <c r="J57" s="180"/>
+      <c r="K57" s="179"/>
+      <c r="L57" s="179"/>
     </row>
     <row r="58" spans="2:12" x14ac:dyDescent="0.25">
       <c r="G58" s="173"/>
@@ -6868,33 +6906,6 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="I58:J58"/>
-    <mergeCell ref="K58:L58"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="K45:L45"/>
-    <mergeCell ref="G57:H57"/>
-    <mergeCell ref="I57:J57"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="K20:L20"/>
     <mergeCell ref="B2:L2"/>
     <mergeCell ref="B18:L18"/>
     <mergeCell ref="G32:H32"/>
@@ -6911,6 +6922,33 @@
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="K58:L58"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="K45:L45"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="K57:L57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -6952,49 +6990,49 @@
     </row>
     <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="27"/>
-      <c r="B2" s="163" t="s">
+      <c r="B2" s="186" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
+      <c r="C2" s="186"/>
+      <c r="D2" s="186"/>
+      <c r="E2" s="186"/>
+      <c r="F2" s="186"/>
+      <c r="G2" s="186"/>
+      <c r="H2" s="186"/>
       <c r="I2" s="27"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="27"/>
       <c r="B3" s="31"/>
-      <c r="C3" s="164" t="s">
+      <c r="C3" s="182" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="177"/>
-      <c r="E3" s="164" t="s">
+      <c r="D3" s="195"/>
+      <c r="E3" s="182" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="177"/>
-      <c r="G3" s="164" t="s">
+      <c r="F3" s="195"/>
+      <c r="G3" s="182" t="s">
         <v>38</v>
       </c>
-      <c r="H3" s="177"/>
+      <c r="H3" s="195"/>
       <c r="I3" s="27"/>
     </row>
     <row r="4" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="27"/>
       <c r="B4" s="31"/>
-      <c r="C4" s="160" t="s">
+      <c r="C4" s="170" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="177"/>
-      <c r="E4" s="178" t="s">
+      <c r="D4" s="195"/>
+      <c r="E4" s="196" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="179"/>
-      <c r="G4" s="160" t="s">
+      <c r="F4" s="197"/>
+      <c r="G4" s="170" t="s">
         <v>46</v>
       </c>
-      <c r="H4" s="160"/>
+      <c r="H4" s="170"/>
       <c r="I4" s="27"/>
     </row>
     <row r="5" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7153,18 +7191,18 @@
       <c r="B14" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="170">
+      <c r="C14" s="179">
         <v>38</v>
       </c>
-      <c r="D14" s="181"/>
-      <c r="E14" s="184">
+      <c r="D14" s="191"/>
+      <c r="E14" s="194">
         <v>38</v>
       </c>
-      <c r="F14" s="181"/>
-      <c r="G14" s="170">
+      <c r="F14" s="191"/>
+      <c r="G14" s="179">
         <v>38</v>
       </c>
-      <c r="H14" s="170"/>
+      <c r="H14" s="179"/>
       <c r="I14" s="27"/>
     </row>
     <row r="15" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7175,11 +7213,11 @@
       <c r="C15" s="173">
         <v>0.55581969851319468</v>
       </c>
-      <c r="D15" s="182"/>
-      <c r="E15" s="209">
+      <c r="D15" s="192"/>
+      <c r="E15" s="220">
         <v>0.54352923406841147</v>
       </c>
-      <c r="F15" s="210"/>
+      <c r="F15" s="221"/>
       <c r="G15" s="173">
         <v>0.55189173576406514</v>
       </c>
@@ -7188,49 +7226,49 @@
     </row>
     <row r="16" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="27"/>
-      <c r="B16" s="163" t="s">
+      <c r="B16" s="186" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="163"/>
-      <c r="D16" s="163"/>
-      <c r="E16" s="163"/>
-      <c r="F16" s="163"/>
-      <c r="G16" s="163"/>
-      <c r="H16" s="163"/>
+      <c r="C16" s="186"/>
+      <c r="D16" s="186"/>
+      <c r="E16" s="186"/>
+      <c r="F16" s="186"/>
+      <c r="G16" s="186"/>
+      <c r="H16" s="186"/>
       <c r="I16" s="27"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="27"/>
       <c r="B17" s="30"/>
-      <c r="C17" s="164" t="s">
+      <c r="C17" s="182" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="177"/>
-      <c r="E17" s="164" t="s">
+      <c r="D17" s="195"/>
+      <c r="E17" s="182" t="s">
         <v>40</v>
       </c>
-      <c r="F17" s="177"/>
-      <c r="G17" s="164" t="s">
+      <c r="F17" s="195"/>
+      <c r="G17" s="182" t="s">
         <v>48</v>
       </c>
-      <c r="H17" s="177"/>
+      <c r="H17" s="195"/>
       <c r="I17" s="27"/>
     </row>
     <row r="18" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="27"/>
       <c r="B18" s="30"/>
-      <c r="C18" s="160" t="s">
+      <c r="C18" s="170" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="177"/>
-      <c r="E18" s="178" t="s">
+      <c r="D18" s="195"/>
+      <c r="E18" s="196" t="s">
         <v>31</v>
       </c>
-      <c r="F18" s="179"/>
-      <c r="G18" s="160" t="s">
+      <c r="F18" s="197"/>
+      <c r="G18" s="170" t="s">
         <v>46</v>
       </c>
-      <c r="H18" s="160"/>
+      <c r="H18" s="170"/>
       <c r="I18" s="27"/>
     </row>
     <row r="19" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7389,18 +7427,18 @@
       <c r="B28" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="170">
+      <c r="C28" s="179">
         <v>38</v>
       </c>
-      <c r="D28" s="181"/>
-      <c r="E28" s="184">
+      <c r="D28" s="191"/>
+      <c r="E28" s="194">
         <v>38</v>
       </c>
-      <c r="F28" s="181"/>
-      <c r="G28" s="170">
+      <c r="F28" s="191"/>
+      <c r="G28" s="179">
         <v>38</v>
       </c>
-      <c r="H28" s="170"/>
+      <c r="H28" s="179"/>
       <c r="I28" s="27"/>
     </row>
     <row r="29" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7408,14 +7446,14 @@
       <c r="B29" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="206">
+      <c r="C29" s="224">
         <v>8.7068576318375279E-2</v>
       </c>
-      <c r="D29" s="205"/>
-      <c r="E29" s="204">
+      <c r="D29" s="223"/>
+      <c r="E29" s="222">
         <v>0.1066523504141621</v>
       </c>
-      <c r="F29" s="205"/>
+      <c r="F29" s="223"/>
       <c r="G29" s="173">
         <v>6.1086704610555098E-2</v>
       </c>
@@ -7424,26 +7462,26 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="27"/>
-      <c r="B30" s="207" t="s">
+      <c r="B30" s="218" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="207"/>
-      <c r="D30" s="207"/>
-      <c r="E30" s="207"/>
-      <c r="F30" s="207"/>
-      <c r="G30" s="207"/>
-      <c r="H30" s="207"/>
+      <c r="C30" s="218"/>
+      <c r="D30" s="218"/>
+      <c r="E30" s="218"/>
+      <c r="F30" s="218"/>
+      <c r="G30" s="218"/>
+      <c r="H30" s="218"/>
       <c r="I30" s="27"/>
     </row>
     <row r="31" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="27"/>
-      <c r="B31" s="208"/>
-      <c r="C31" s="208"/>
-      <c r="D31" s="208"/>
-      <c r="E31" s="208"/>
-      <c r="F31" s="208"/>
-      <c r="G31" s="208"/>
-      <c r="H31" s="208"/>
+      <c r="B31" s="219"/>
+      <c r="C31" s="219"/>
+      <c r="D31" s="219"/>
+      <c r="E31" s="219"/>
+      <c r="F31" s="219"/>
+      <c r="G31" s="219"/>
+      <c r="H31" s="219"/>
       <c r="I31" s="27"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -7470,6 +7508,17 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="E4:F4"/>
@@ -7486,17 +7535,6 @@
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -7545,12 +7583,12 @@
     <row r="2" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="104"/>
-      <c r="C2" s="161" t="s">
+      <c r="C2" s="171" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="161"/>
-      <c r="E2" s="161"/>
-      <c r="F2" s="161"/>
+      <c r="D2" s="171"/>
+      <c r="E2" s="171"/>
+      <c r="F2" s="171"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
     </row>
@@ -8550,17 +8588,17 @@
     </row>
     <row r="2" spans="1:17" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27"/>
-      <c r="B2" s="162" t="s">
+      <c r="B2" s="185" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
-      <c r="I2" s="163"/>
-      <c r="J2" s="163"/>
+      <c r="C2" s="186"/>
+      <c r="D2" s="186"/>
+      <c r="E2" s="186"/>
+      <c r="F2" s="186"/>
+      <c r="G2" s="186"/>
+      <c r="H2" s="186"/>
+      <c r="I2" s="186"/>
+      <c r="J2" s="186"/>
       <c r="K2" s="27"/>
       <c r="L2" s="27"/>
       <c r="M2" s="27"/>
@@ -8571,22 +8609,22 @@
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="27"/>
       <c r="B3" s="31"/>
-      <c r="C3" s="164" t="s">
+      <c r="C3" s="182" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="177"/>
-      <c r="E3" s="164" t="s">
+      <c r="D3" s="195"/>
+      <c r="E3" s="182" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="177"/>
-      <c r="G3" s="180" t="s">
+      <c r="F3" s="195"/>
+      <c r="G3" s="198" t="s">
         <v>87</v>
       </c>
-      <c r="H3" s="211"/>
-      <c r="I3" s="164" t="s">
+      <c r="H3" s="225"/>
+      <c r="I3" s="182" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="160"/>
+      <c r="J3" s="170"/>
       <c r="K3" s="27"/>
       <c r="L3" s="27"/>
       <c r="M3" s="27"/>
@@ -8597,22 +8635,22 @@
     <row r="4" spans="1:17" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="27"/>
       <c r="B4" s="31"/>
-      <c r="C4" s="169" t="s">
+      <c r="C4" s="176" t="s">
         <v>84</v>
       </c>
-      <c r="D4" s="177"/>
-      <c r="E4" s="178" t="s">
+      <c r="D4" s="195"/>
+      <c r="E4" s="196" t="s">
         <v>86</v>
       </c>
-      <c r="F4" s="179"/>
-      <c r="G4" s="178" t="s">
+      <c r="F4" s="197"/>
+      <c r="G4" s="196" t="s">
         <v>88</v>
       </c>
-      <c r="H4" s="179"/>
-      <c r="I4" s="178" t="s">
+      <c r="H4" s="197"/>
+      <c r="I4" s="196" t="s">
         <v>85</v>
       </c>
-      <c r="J4" s="160"/>
+      <c r="J4" s="170"/>
       <c r="K4" s="27"/>
       <c r="L4" s="27"/>
       <c r="M4" s="27"/>
@@ -8783,22 +8821,22 @@
       <c r="B10" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="170">
+      <c r="C10" s="179">
         <v>31</v>
       </c>
-      <c r="D10" s="181"/>
-      <c r="E10" s="170">
+      <c r="D10" s="191"/>
+      <c r="E10" s="179">
         <v>32</v>
       </c>
-      <c r="F10" s="181"/>
-      <c r="G10" s="184">
+      <c r="F10" s="191"/>
+      <c r="G10" s="194">
         <v>21</v>
       </c>
-      <c r="H10" s="181"/>
-      <c r="I10" s="170">
+      <c r="H10" s="191"/>
+      <c r="I10" s="179">
         <v>33</v>
       </c>
-      <c r="J10" s="170"/>
+      <c r="J10" s="179"/>
       <c r="K10" s="27"/>
       <c r="L10" s="27"/>
       <c r="M10" s="27"/>
@@ -8815,17 +8853,17 @@
         <f>N11</f>
         <v>0.61571897814696952</v>
       </c>
-      <c r="D11" s="182"/>
-      <c r="E11" s="183">
+      <c r="D11" s="192"/>
+      <c r="E11" s="193">
         <f>O11</f>
         <v>0.72486496224438524</v>
       </c>
-      <c r="F11" s="182"/>
-      <c r="G11" s="183">
+      <c r="F11" s="192"/>
+      <c r="G11" s="193">
         <f>P11</f>
         <v>0.79096913931575263</v>
       </c>
-      <c r="H11" s="182"/>
+      <c r="H11" s="192"/>
       <c r="I11" s="173">
         <f>Q11</f>
         <v>0.72277433456881901</v>
@@ -8849,17 +8887,17 @@
     </row>
     <row r="12" spans="1:17" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="27"/>
-      <c r="B12" s="185" t="s">
+      <c r="B12" s="187" t="s">
         <v>101</v>
       </c>
-      <c r="C12" s="186"/>
-      <c r="D12" s="186"/>
-      <c r="E12" s="186"/>
-      <c r="F12" s="186"/>
-      <c r="G12" s="186"/>
-      <c r="H12" s="186"/>
-      <c r="I12" s="186"/>
-      <c r="J12" s="186"/>
+      <c r="C12" s="188"/>
+      <c r="D12" s="188"/>
+      <c r="E12" s="188"/>
+      <c r="F12" s="188"/>
+      <c r="G12" s="188"/>
+      <c r="H12" s="188"/>
+      <c r="I12" s="188"/>
+      <c r="J12" s="188"/>
       <c r="K12" s="27"/>
       <c r="L12" s="27"/>
       <c r="M12" s="27"/>
@@ -8870,22 +8908,22 @@
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="27"/>
       <c r="B13" s="30"/>
-      <c r="C13" s="164" t="s">
+      <c r="C13" s="182" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="177"/>
-      <c r="E13" s="164" t="s">
+      <c r="D13" s="195"/>
+      <c r="E13" s="182" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="177"/>
-      <c r="G13" s="180" t="s">
+      <c r="F13" s="195"/>
+      <c r="G13" s="198" t="s">
         <v>87</v>
       </c>
-      <c r="H13" s="211"/>
-      <c r="I13" s="164" t="s">
+      <c r="H13" s="225"/>
+      <c r="I13" s="182" t="s">
         <v>38</v>
       </c>
-      <c r="J13" s="160"/>
+      <c r="J13" s="170"/>
       <c r="K13" s="27"/>
       <c r="L13" s="27"/>
       <c r="M13" s="27"/>
@@ -8896,22 +8934,22 @@
     <row r="14" spans="1:17" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="27"/>
       <c r="B14" s="30"/>
-      <c r="C14" s="160" t="s">
+      <c r="C14" s="170" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="177"/>
-      <c r="E14" s="178" t="s">
+      <c r="D14" s="195"/>
+      <c r="E14" s="196" t="s">
         <v>86</v>
       </c>
-      <c r="F14" s="179"/>
-      <c r="G14" s="178" t="s">
+      <c r="F14" s="197"/>
+      <c r="G14" s="196" t="s">
         <v>88</v>
       </c>
-      <c r="H14" s="179"/>
-      <c r="I14" s="178" t="s">
+      <c r="H14" s="197"/>
+      <c r="I14" s="196" t="s">
         <v>85</v>
       </c>
-      <c r="J14" s="160"/>
+      <c r="J14" s="170"/>
       <c r="K14" s="27"/>
       <c r="L14" s="27"/>
       <c r="M14" s="27"/>
@@ -9082,22 +9120,22 @@
       <c r="B20" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="170">
+      <c r="C20" s="179">
         <v>31</v>
       </c>
-      <c r="D20" s="181"/>
-      <c r="E20" s="170">
+      <c r="D20" s="191"/>
+      <c r="E20" s="179">
         <v>32</v>
       </c>
-      <c r="F20" s="181"/>
-      <c r="G20" s="184">
+      <c r="F20" s="191"/>
+      <c r="G20" s="194">
         <v>21</v>
       </c>
-      <c r="H20" s="181"/>
-      <c r="I20" s="170">
+      <c r="H20" s="191"/>
+      <c r="I20" s="179">
         <v>33</v>
       </c>
-      <c r="J20" s="170"/>
+      <c r="J20" s="179"/>
       <c r="K20" s="27"/>
       <c r="L20" s="27"/>
       <c r="M20" s="27"/>
@@ -9114,18 +9152,18 @@
         <f>N21</f>
         <v>0.12235556050138582</v>
       </c>
-      <c r="D21" s="182"/>
-      <c r="E21" s="183">
+      <c r="D21" s="192"/>
+      <c r="E21" s="193">
         <f>O21</f>
         <v>0.14817255106920282</v>
       </c>
-      <c r="F21" s="182"/>
-      <c r="G21" s="183">
+      <c r="F21" s="192"/>
+      <c r="G21" s="193">
         <f>P21</f>
         <v>0.20221725039002678</v>
       </c>
-      <c r="H21" s="182"/>
-      <c r="I21" s="183">
+      <c r="H21" s="192"/>
+      <c r="I21" s="193">
         <f>Q21</f>
         <v>0.13282978602147921</v>
       </c>
@@ -9148,17 +9186,17 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="27"/>
-      <c r="B22" s="207" t="s">
+      <c r="B22" s="218" t="s">
         <v>90</v>
       </c>
-      <c r="C22" s="207"/>
-      <c r="D22" s="207"/>
-      <c r="E22" s="207"/>
-      <c r="F22" s="207"/>
-      <c r="G22" s="207"/>
-      <c r="H22" s="207"/>
-      <c r="I22" s="207"/>
-      <c r="J22" s="207"/>
+      <c r="C22" s="218"/>
+      <c r="D22" s="218"/>
+      <c r="E22" s="218"/>
+      <c r="F22" s="218"/>
+      <c r="G22" s="218"/>
+      <c r="H22" s="218"/>
+      <c r="I22" s="218"/>
+      <c r="J22" s="218"/>
       <c r="K22" s="27"/>
       <c r="L22" s="27"/>
       <c r="M22" s="27"/>
@@ -9168,15 +9206,15 @@
     </row>
     <row r="23" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="27"/>
-      <c r="B23" s="208"/>
-      <c r="C23" s="208"/>
-      <c r="D23" s="208"/>
-      <c r="E23" s="208"/>
-      <c r="F23" s="208"/>
-      <c r="G23" s="208"/>
-      <c r="H23" s="208"/>
-      <c r="I23" s="208"/>
-      <c r="J23" s="208"/>
+      <c r="B23" s="219"/>
+      <c r="C23" s="219"/>
+      <c r="D23" s="219"/>
+      <c r="E23" s="219"/>
+      <c r="F23" s="219"/>
+      <c r="G23" s="219"/>
+      <c r="H23" s="219"/>
+      <c r="I23" s="219"/>
+      <c r="J23" s="219"/>
       <c r="K23" s="27"/>
       <c r="L23" s="27"/>
       <c r="M23" s="27"/>
@@ -9216,6 +9254,27 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="B12:J12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
     <mergeCell ref="I13:J13"/>
     <mergeCell ref="B22:J23"/>
     <mergeCell ref="C20:D20"/>
@@ -9230,27 +9289,6 @@
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="I14:J14"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="B12:J12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10231,89 +10269,89 @@
     </row>
     <row r="2" spans="1:17" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27"/>
-      <c r="B2" s="162" t="s">
+      <c r="B2" s="185" t="s">
         <v>99</v>
       </c>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
-      <c r="I2" s="163"/>
-      <c r="J2" s="163"/>
-      <c r="K2" s="163"/>
-      <c r="L2" s="163"/>
+      <c r="C2" s="186"/>
+      <c r="D2" s="186"/>
+      <c r="E2" s="186"/>
+      <c r="F2" s="186"/>
+      <c r="G2" s="186"/>
+      <c r="H2" s="186"/>
+      <c r="I2" s="186"/>
+      <c r="J2" s="186"/>
+      <c r="K2" s="186"/>
+      <c r="L2" s="186"/>
       <c r="M2" s="27"/>
       <c r="N2" s="7"/>
     </row>
     <row r="3" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27"/>
       <c r="B3" s="138"/>
-      <c r="C3" s="166" t="s">
+      <c r="C3" s="172" t="s">
         <v>123</v>
       </c>
-      <c r="D3" s="166"/>
-      <c r="E3" s="166"/>
-      <c r="F3" s="166"/>
-      <c r="G3" s="166"/>
-      <c r="H3" s="166"/>
-      <c r="I3" s="166"/>
-      <c r="J3" s="166"/>
-      <c r="K3" s="166"/>
-      <c r="L3" s="166"/>
+      <c r="D3" s="172"/>
+      <c r="E3" s="172"/>
+      <c r="F3" s="172"/>
+      <c r="G3" s="172"/>
+      <c r="H3" s="172"/>
+      <c r="I3" s="172"/>
+      <c r="J3" s="172"/>
+      <c r="K3" s="172"/>
+      <c r="L3" s="172"/>
       <c r="M3" s="27"/>
       <c r="N3" s="7"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="27"/>
       <c r="B4" s="30"/>
-      <c r="C4" s="164" t="s">
+      <c r="C4" s="182" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="165"/>
-      <c r="E4" s="164" t="s">
+      <c r="D4" s="183"/>
+      <c r="E4" s="182" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="165"/>
-      <c r="G4" s="164" t="s">
+      <c r="F4" s="183"/>
+      <c r="G4" s="182" t="s">
         <v>38</v>
       </c>
-      <c r="H4" s="165"/>
-      <c r="I4" s="164" t="s">
+      <c r="H4" s="183"/>
+      <c r="I4" s="182" t="s">
         <v>39</v>
       </c>
-      <c r="J4" s="165"/>
-      <c r="K4" s="164" t="s">
+      <c r="J4" s="183"/>
+      <c r="K4" s="182" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="160"/>
+      <c r="L4" s="170"/>
       <c r="M4" s="27"/>
       <c r="N4" s="7"/>
     </row>
     <row r="5" spans="1:17" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="27"/>
       <c r="B5" s="30"/>
-      <c r="C5" s="160" t="s">
+      <c r="C5" s="170" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="165"/>
-      <c r="E5" s="167" t="s">
+      <c r="D5" s="183"/>
+      <c r="E5" s="178" t="s">
         <v>124</v>
       </c>
-      <c r="F5" s="168"/>
-      <c r="G5" s="169" t="s">
+      <c r="F5" s="177"/>
+      <c r="G5" s="176" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="168"/>
-      <c r="I5" s="167" t="s">
+      <c r="H5" s="177"/>
+      <c r="I5" s="178" t="s">
         <v>125</v>
       </c>
-      <c r="J5" s="168"/>
-      <c r="K5" s="169" t="s">
+      <c r="J5" s="177"/>
+      <c r="K5" s="176" t="s">
         <v>126</v>
       </c>
-      <c r="L5" s="169"/>
+      <c r="L5" s="176"/>
       <c r="M5" s="27"/>
       <c r="N5" s="7"/>
     </row>
@@ -10516,26 +10554,26 @@
       <c r="B12" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="170">
+      <c r="C12" s="179">
         <v>38</v>
       </c>
-      <c r="D12" s="171"/>
-      <c r="E12" s="172">
+      <c r="D12" s="180"/>
+      <c r="E12" s="181">
         <v>38</v>
       </c>
-      <c r="F12" s="171"/>
-      <c r="G12" s="170">
+      <c r="F12" s="180"/>
+      <c r="G12" s="179">
         <v>38</v>
       </c>
-      <c r="H12" s="171"/>
-      <c r="I12" s="172">
+      <c r="H12" s="180"/>
+      <c r="I12" s="181">
         <v>38</v>
       </c>
-      <c r="J12" s="171"/>
-      <c r="K12" s="170">
+      <c r="J12" s="180"/>
+      <c r="K12" s="179">
         <v>38</v>
       </c>
-      <c r="L12" s="170"/>
+      <c r="L12" s="179"/>
       <c r="M12" s="27"/>
       <c r="N12" s="7"/>
     </row>
@@ -10581,36 +10619,36 @@
     </row>
     <row r="14" spans="1:17" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="27"/>
-      <c r="B14" s="162" t="s">
+      <c r="B14" s="185" t="s">
         <v>98</v>
       </c>
-      <c r="C14" s="163"/>
-      <c r="D14" s="163"/>
-      <c r="E14" s="163"/>
-      <c r="F14" s="163"/>
-      <c r="G14" s="163"/>
-      <c r="H14" s="163"/>
-      <c r="I14" s="163"/>
-      <c r="J14" s="163"/>
-      <c r="K14" s="163"/>
-      <c r="L14" s="163"/>
+      <c r="C14" s="186"/>
+      <c r="D14" s="186"/>
+      <c r="E14" s="186"/>
+      <c r="F14" s="186"/>
+      <c r="G14" s="186"/>
+      <c r="H14" s="186"/>
+      <c r="I14" s="186"/>
+      <c r="J14" s="186"/>
+      <c r="K14" s="186"/>
+      <c r="L14" s="186"/>
       <c r="M14" s="27"/>
     </row>
     <row r="15" spans="1:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="27"/>
       <c r="B15" s="138"/>
-      <c r="C15" s="166" t="s">
+      <c r="C15" s="172" t="s">
         <v>123</v>
       </c>
-      <c r="D15" s="166"/>
-      <c r="E15" s="166"/>
-      <c r="F15" s="166"/>
-      <c r="G15" s="166"/>
-      <c r="H15" s="166"/>
-      <c r="I15" s="166"/>
-      <c r="J15" s="166"/>
-      <c r="K15" s="166"/>
-      <c r="L15" s="166"/>
+      <c r="D15" s="172"/>
+      <c r="E15" s="172"/>
+      <c r="F15" s="172"/>
+      <c r="G15" s="172"/>
+      <c r="H15" s="172"/>
+      <c r="I15" s="172"/>
+      <c r="J15" s="172"/>
+      <c r="K15" s="172"/>
+      <c r="L15" s="172"/>
       <c r="M15" s="27"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -10620,18 +10658,18 @@
       <c r="D16" s="24"/>
       <c r="E16" s="17"/>
       <c r="F16" s="52"/>
-      <c r="G16" s="164" t="s">
+      <c r="G16" s="182" t="s">
         <v>41</v>
       </c>
-      <c r="H16" s="165"/>
-      <c r="I16" s="164" t="s">
+      <c r="H16" s="183"/>
+      <c r="I16" s="182" t="s">
         <v>42</v>
       </c>
-      <c r="J16" s="165"/>
-      <c r="K16" s="164" t="s">
+      <c r="J16" s="183"/>
+      <c r="K16" s="182" t="s">
         <v>43</v>
       </c>
-      <c r="L16" s="160"/>
+      <c r="L16" s="170"/>
       <c r="M16" s="27"/>
     </row>
     <row r="17" spans="1:17" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10641,18 +10679,18 @@
       <c r="D17" s="24"/>
       <c r="E17" s="17"/>
       <c r="F17" s="52"/>
-      <c r="G17" s="176" t="s">
+      <c r="G17" s="184" t="s">
         <v>5</v>
       </c>
-      <c r="H17" s="165"/>
-      <c r="I17" s="167" t="s">
+      <c r="H17" s="183"/>
+      <c r="I17" s="178" t="s">
         <v>127</v>
       </c>
-      <c r="J17" s="168"/>
-      <c r="K17" s="169" t="s">
+      <c r="J17" s="177"/>
+      <c r="K17" s="176" t="s">
         <v>128</v>
       </c>
-      <c r="L17" s="169"/>
+      <c r="L17" s="176"/>
       <c r="M17" s="27"/>
     </row>
     <row r="18" spans="1:17" ht="42" customHeight="1" x14ac:dyDescent="0.25">
@@ -10824,18 +10862,18 @@
       <c r="D24" s="20"/>
       <c r="E24" s="20"/>
       <c r="F24" s="54"/>
-      <c r="G24" s="170">
+      <c r="G24" s="179">
         <v>38</v>
       </c>
-      <c r="H24" s="171"/>
-      <c r="I24" s="172">
+      <c r="H24" s="180"/>
+      <c r="I24" s="181">
         <v>38</v>
       </c>
-      <c r="J24" s="171"/>
-      <c r="K24" s="170">
+      <c r="J24" s="180"/>
+      <c r="K24" s="179">
         <v>38</v>
       </c>
-      <c r="L24" s="170"/>
+      <c r="L24" s="179"/>
       <c r="M24" s="27"/>
     </row>
     <row r="25" spans="1:17" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -10961,12 +10999,12 @@
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B37" s="24"/>
-      <c r="G37" s="169"/>
-      <c r="H37" s="168"/>
-      <c r="I37" s="167"/>
-      <c r="J37" s="168"/>
-      <c r="K37" s="169"/>
-      <c r="L37" s="169"/>
+      <c r="G37" s="176"/>
+      <c r="H37" s="177"/>
+      <c r="I37" s="178"/>
+      <c r="J37" s="177"/>
+      <c r="K37" s="176"/>
+      <c r="L37" s="176"/>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B38" s="24"/>
@@ -11065,12 +11103,12 @@
       <c r="L48" s="19"/>
     </row>
     <row r="49" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G49" s="170"/>
-      <c r="H49" s="171"/>
-      <c r="I49" s="172"/>
-      <c r="J49" s="171"/>
-      <c r="K49" s="170"/>
-      <c r="L49" s="170"/>
+      <c r="G49" s="179"/>
+      <c r="H49" s="180"/>
+      <c r="I49" s="181"/>
+      <c r="J49" s="180"/>
+      <c r="K49" s="179"/>
+      <c r="L49" s="179"/>
     </row>
     <row r="50" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G50" s="173"/>
@@ -11082,6 +11120,35 @@
     </row>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="C3:L3"/>
+    <mergeCell ref="B14:L14"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="K17:L17"/>
     <mergeCell ref="C15:L15"/>
     <mergeCell ref="G50:H50"/>
     <mergeCell ref="I50:J50"/>
@@ -11098,35 +11165,6 @@
     <mergeCell ref="G25:H25"/>
     <mergeCell ref="I25:J25"/>
     <mergeCell ref="K25:L25"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="B14:L14"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="C3:L3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -11169,15 +11207,15 @@
     </row>
     <row r="2" spans="1:14" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27"/>
-      <c r="B2" s="162" t="s">
+      <c r="B2" s="185" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
+      <c r="C2" s="186"/>
+      <c r="D2" s="186"/>
+      <c r="E2" s="186"/>
+      <c r="F2" s="186"/>
+      <c r="G2" s="186"/>
+      <c r="H2" s="186"/>
       <c r="I2" s="27"/>
       <c r="J2" s="27"/>
       <c r="K2" s="27"/>
@@ -11188,18 +11226,18 @@
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="27"/>
       <c r="B3" s="31"/>
-      <c r="C3" s="164" t="s">
+      <c r="C3" s="182" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="177"/>
-      <c r="E3" s="164" t="s">
+      <c r="D3" s="195"/>
+      <c r="E3" s="182" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="177"/>
-      <c r="G3" s="180" t="s">
+      <c r="F3" s="195"/>
+      <c r="G3" s="198" t="s">
         <v>87</v>
       </c>
-      <c r="H3" s="164"/>
+      <c r="H3" s="182"/>
       <c r="I3" s="27"/>
       <c r="J3" s="27"/>
       <c r="K3" s="27"/>
@@ -11210,18 +11248,18 @@
     <row r="4" spans="1:14" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="27"/>
       <c r="B4" s="31"/>
-      <c r="C4" s="169" t="s">
+      <c r="C4" s="176" t="s">
         <v>84</v>
       </c>
-      <c r="D4" s="177"/>
-      <c r="E4" s="178" t="s">
+      <c r="D4" s="195"/>
+      <c r="E4" s="196" t="s">
         <v>131</v>
       </c>
-      <c r="F4" s="179"/>
-      <c r="G4" s="178" t="s">
+      <c r="F4" s="197"/>
+      <c r="G4" s="196" t="s">
         <v>132</v>
       </c>
-      <c r="H4" s="169"/>
+      <c r="H4" s="176"/>
       <c r="I4" s="27"/>
       <c r="J4" s="27"/>
       <c r="K4" s="27"/>
@@ -11374,18 +11412,18 @@
       <c r="B10" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="170">
+      <c r="C10" s="179">
         <v>31</v>
       </c>
-      <c r="D10" s="181"/>
-      <c r="E10" s="170">
+      <c r="D10" s="191"/>
+      <c r="E10" s="179">
         <v>32</v>
       </c>
-      <c r="F10" s="181"/>
-      <c r="G10" s="184">
+      <c r="F10" s="191"/>
+      <c r="G10" s="194">
         <v>21</v>
       </c>
-      <c r="H10" s="170"/>
+      <c r="H10" s="179"/>
       <c r="I10" s="27"/>
       <c r="J10" s="27"/>
       <c r="K10" s="27"/>
@@ -11402,13 +11440,13 @@
         <f>L11</f>
         <v>0.61571897814696952</v>
       </c>
-      <c r="D11" s="182"/>
-      <c r="E11" s="183">
+      <c r="D11" s="192"/>
+      <c r="E11" s="193">
         <f>M11</f>
         <v>0.7417219375190941</v>
       </c>
-      <c r="F11" s="182"/>
-      <c r="G11" s="183">
+      <c r="F11" s="192"/>
+      <c r="G11" s="193">
         <f>N11</f>
         <v>0.80466929780955043</v>
       </c>
@@ -11428,15 +11466,15 @@
     </row>
     <row r="12" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="27"/>
-      <c r="B12" s="185" t="s">
+      <c r="B12" s="187" t="s">
         <v>130</v>
       </c>
-      <c r="C12" s="186"/>
-      <c r="D12" s="186"/>
-      <c r="E12" s="186"/>
-      <c r="F12" s="186"/>
-      <c r="G12" s="186"/>
-      <c r="H12" s="186"/>
+      <c r="C12" s="188"/>
+      <c r="D12" s="188"/>
+      <c r="E12" s="188"/>
+      <c r="F12" s="188"/>
+      <c r="G12" s="188"/>
+      <c r="H12" s="188"/>
       <c r="I12" s="27"/>
       <c r="J12" s="27"/>
       <c r="K12" s="27"/>
@@ -11447,18 +11485,18 @@
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="27"/>
       <c r="B13" s="30"/>
-      <c r="C13" s="164" t="s">
+      <c r="C13" s="182" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="177"/>
-      <c r="E13" s="164" t="s">
+      <c r="D13" s="195"/>
+      <c r="E13" s="182" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="177"/>
-      <c r="G13" s="180" t="s">
+      <c r="F13" s="195"/>
+      <c r="G13" s="198" t="s">
         <v>87</v>
       </c>
-      <c r="H13" s="164"/>
+      <c r="H13" s="182"/>
       <c r="I13" s="27"/>
       <c r="J13" s="27"/>
       <c r="K13" s="27"/>
@@ -11469,18 +11507,18 @@
     <row r="14" spans="1:14" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="27"/>
       <c r="B14" s="30"/>
-      <c r="C14" s="169" t="s">
+      <c r="C14" s="176" t="s">
         <v>84</v>
       </c>
-      <c r="D14" s="177"/>
-      <c r="E14" s="178" t="s">
+      <c r="D14" s="195"/>
+      <c r="E14" s="196" t="s">
         <v>131</v>
       </c>
-      <c r="F14" s="179"/>
-      <c r="G14" s="178" t="s">
+      <c r="F14" s="197"/>
+      <c r="G14" s="196" t="s">
         <v>132</v>
       </c>
-      <c r="H14" s="169"/>
+      <c r="H14" s="176"/>
       <c r="I14" s="27"/>
       <c r="J14" s="27"/>
       <c r="K14" s="27"/>
@@ -11633,18 +11671,18 @@
       <c r="B20" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="170">
+      <c r="C20" s="179">
         <v>31</v>
       </c>
-      <c r="D20" s="181"/>
-      <c r="E20" s="170">
+      <c r="D20" s="191"/>
+      <c r="E20" s="179">
         <v>32</v>
       </c>
-      <c r="F20" s="181"/>
-      <c r="G20" s="184">
+      <c r="F20" s="191"/>
+      <c r="G20" s="194">
         <v>21</v>
       </c>
-      <c r="H20" s="170"/>
+      <c r="H20" s="179"/>
       <c r="I20" s="27"/>
       <c r="J20" s="27"/>
       <c r="K20" s="27"/>
@@ -11661,13 +11699,13 @@
         <f>L21</f>
         <v>0.12235556050138582</v>
       </c>
-      <c r="D21" s="182"/>
-      <c r="E21" s="183">
+      <c r="D21" s="192"/>
+      <c r="E21" s="193">
         <f>M21</f>
         <v>0.15210459418202643</v>
       </c>
-      <c r="F21" s="182"/>
-      <c r="G21" s="183">
+      <c r="F21" s="192"/>
+      <c r="G21" s="193">
         <f>N21</f>
         <v>0.26204031407125944</v>
       </c>
@@ -11687,28 +11725,28 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="27"/>
-      <c r="B22" s="187" t="s">
+      <c r="B22" s="189" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="187"/>
-      <c r="D22" s="187"/>
-      <c r="E22" s="187"/>
-      <c r="F22" s="187"/>
-      <c r="G22" s="187"/>
-      <c r="H22" s="187"/>
+      <c r="C22" s="189"/>
+      <c r="D22" s="189"/>
+      <c r="E22" s="189"/>
+      <c r="F22" s="189"/>
+      <c r="G22" s="189"/>
+      <c r="H22" s="189"/>
       <c r="I22" s="27"/>
       <c r="J22" s="27"/>
       <c r="K22" s="27"/>
     </row>
     <row r="23" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="27"/>
-      <c r="B23" s="188"/>
-      <c r="C23" s="188"/>
-      <c r="D23" s="188"/>
-      <c r="E23" s="188"/>
-      <c r="F23" s="188"/>
-      <c r="G23" s="188"/>
-      <c r="H23" s="188"/>
+      <c r="B23" s="190"/>
+      <c r="C23" s="190"/>
+      <c r="D23" s="190"/>
+      <c r="E23" s="190"/>
+      <c r="F23" s="190"/>
+      <c r="G23" s="190"/>
+      <c r="H23" s="190"/>
       <c r="I23" s="27"/>
       <c r="J23" s="27"/>
       <c r="K23" s="27"/>
@@ -11741,6 +11779,17 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B12:H12"/>
     <mergeCell ref="B22:H23"/>
@@ -11757,17 +11806,6 @@
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -11811,61 +11849,61 @@
     </row>
     <row r="2" spans="1:16" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27"/>
-      <c r="B2" s="162" t="s">
+      <c r="B2" s="185" t="s">
         <v>102</v>
       </c>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
-      <c r="I2" s="163"/>
-      <c r="J2" s="163"/>
+      <c r="C2" s="186"/>
+      <c r="D2" s="186"/>
+      <c r="E2" s="186"/>
+      <c r="F2" s="186"/>
+      <c r="G2" s="186"/>
+      <c r="H2" s="186"/>
+      <c r="I2" s="186"/>
+      <c r="J2" s="186"/>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="27"/>
       <c r="B3" s="31"/>
-      <c r="C3" s="164" t="s">
+      <c r="C3" s="182" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="177"/>
-      <c r="E3" s="164" t="s">
+      <c r="D3" s="195"/>
+      <c r="E3" s="182" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="177"/>
-      <c r="G3" s="180" t="s">
+      <c r="F3" s="195"/>
+      <c r="G3" s="198" t="s">
         <v>38</v>
       </c>
-      <c r="H3" s="177"/>
-      <c r="I3" s="164" t="s">
+      <c r="H3" s="195"/>
+      <c r="I3" s="182" t="s">
         <v>39</v>
       </c>
-      <c r="J3" s="160"/>
+      <c r="J3" s="170"/>
       <c r="K3" s="27"/>
       <c r="L3" s="7"/>
     </row>
     <row r="4" spans="1:16" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="27"/>
       <c r="B4" s="31"/>
-      <c r="C4" s="160" t="s">
+      <c r="C4" s="170" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="177"/>
-      <c r="E4" s="178" t="s">
+      <c r="D4" s="195"/>
+      <c r="E4" s="196" t="s">
         <v>139</v>
       </c>
-      <c r="F4" s="179"/>
-      <c r="G4" s="178" t="s">
+      <c r="F4" s="197"/>
+      <c r="G4" s="196" t="s">
         <v>137</v>
       </c>
-      <c r="H4" s="177"/>
-      <c r="I4" s="169" t="s">
+      <c r="H4" s="195"/>
+      <c r="I4" s="176" t="s">
         <v>138</v>
       </c>
-      <c r="J4" s="160"/>
+      <c r="J4" s="170"/>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
     </row>
@@ -12048,22 +12086,22 @@
       <c r="B12" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="170">
+      <c r="C12" s="179">
         <v>38</v>
       </c>
-      <c r="D12" s="181"/>
-      <c r="E12" s="184">
+      <c r="D12" s="191"/>
+      <c r="E12" s="194">
         <v>38</v>
       </c>
-      <c r="F12" s="181"/>
-      <c r="G12" s="184">
+      <c r="F12" s="191"/>
+      <c r="G12" s="194">
         <v>38</v>
       </c>
-      <c r="H12" s="181"/>
-      <c r="I12" s="170">
+      <c r="H12" s="191"/>
+      <c r="I12" s="179">
         <v>38</v>
       </c>
-      <c r="J12" s="170"/>
+      <c r="J12" s="179"/>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
     </row>
@@ -12076,17 +12114,17 @@
         <f>M13</f>
         <v>0.3032675605879514</v>
       </c>
-      <c r="D13" s="182"/>
-      <c r="E13" s="183">
+      <c r="D13" s="192"/>
+      <c r="E13" s="193">
         <f>N13</f>
         <v>0.43858138193669671</v>
       </c>
-      <c r="F13" s="182"/>
-      <c r="G13" s="183">
+      <c r="F13" s="192"/>
+      <c r="G13" s="193">
         <f>O13</f>
         <v>0.44569213309189742</v>
       </c>
-      <c r="H13" s="182"/>
+      <c r="H13" s="192"/>
       <c r="I13" s="173">
         <f>P13</f>
         <v>0.45380565810102486</v>
@@ -12109,15 +12147,15 @@
     </row>
     <row r="14" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="27"/>
-      <c r="B14" s="189" t="s">
+      <c r="B14" s="199" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="189"/>
-      <c r="D14" s="189"/>
-      <c r="E14" s="189"/>
-      <c r="F14" s="189"/>
-      <c r="G14" s="189"/>
-      <c r="H14" s="189"/>
+      <c r="C14" s="199"/>
+      <c r="D14" s="199"/>
+      <c r="E14" s="199"/>
+      <c r="F14" s="199"/>
+      <c r="G14" s="199"/>
+      <c r="H14" s="199"/>
       <c r="I14" s="27"/>
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
@@ -12193,11 +12231,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="B2:J2"/>
     <mergeCell ref="B14:H14"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
@@ -12211,6 +12244,11 @@
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="B2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -12262,14 +12300,14 @@
     </row>
     <row r="2" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
-      <c r="B2" s="190" t="s">
+      <c r="B2" s="200" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="190"/>
-      <c r="D2" s="190"/>
-      <c r="E2" s="190"/>
-      <c r="F2" s="190"/>
-      <c r="G2" s="190"/>
+      <c r="C2" s="200"/>
+      <c r="D2" s="200"/>
+      <c r="E2" s="200"/>
+      <c r="F2" s="200"/>
+      <c r="G2" s="200"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
     </row>
@@ -12319,14 +12357,14 @@
     </row>
     <row r="5" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
-      <c r="B5" s="160" t="s">
+      <c r="B5" s="170" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="160"/>
-      <c r="D5" s="160"/>
-      <c r="E5" s="160"/>
-      <c r="F5" s="160"/>
-      <c r="G5" s="160"/>
+      <c r="C5" s="170"/>
+      <c r="D5" s="170"/>
+      <c r="E5" s="170"/>
+      <c r="F5" s="170"/>
+      <c r="G5" s="170"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
     </row>
@@ -12447,14 +12485,14 @@
     </row>
     <row r="11" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
-      <c r="B11" s="160" t="s">
+      <c r="B11" s="170" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="160"/>
-      <c r="D11" s="160"/>
-      <c r="E11" s="160"/>
-      <c r="F11" s="160"/>
-      <c r="G11" s="160"/>
+      <c r="C11" s="170"/>
+      <c r="D11" s="170"/>
+      <c r="E11" s="170"/>
+      <c r="F11" s="170"/>
+      <c r="G11" s="170"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
     </row>
@@ -12658,13 +12696,13 @@
     <row r="2" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="98"/>
-      <c r="C2" s="161" t="s">
+      <c r="C2" s="171" t="s">
         <v>144</v>
       </c>
-      <c r="D2" s="193"/>
-      <c r="E2" s="193"/>
-      <c r="F2" s="193"/>
-      <c r="G2" s="193"/>
+      <c r="D2" s="203"/>
+      <c r="E2" s="203"/>
+      <c r="F2" s="203"/>
+      <c r="G2" s="203"/>
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="1:8" s="77" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -12689,20 +12727,20 @@
       <c r="A4" s="96"/>
       <c r="B4" s="117"/>
       <c r="C4" s="97"/>
-      <c r="D4" s="169" t="s">
+      <c r="D4" s="176" t="s">
         <v>94</v>
       </c>
-      <c r="E4" s="169"/>
-      <c r="F4" s="169"/>
-      <c r="G4" s="169"/>
+      <c r="E4" s="176"/>
+      <c r="F4" s="176"/>
+      <c r="G4" s="176"/>
       <c r="H4" s="96"/>
     </row>
     <row r="5" spans="1:8" s="77" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="96"/>
-      <c r="B5" s="169" t="s">
+      <c r="B5" s="176" t="s">
         <v>140</v>
       </c>
-      <c r="C5" s="169"/>
+      <c r="C5" s="176"/>
       <c r="D5" s="139">
         <v>0.02</v>
       </c>
@@ -12719,7 +12757,7 @@
     </row>
     <row r="6" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
-      <c r="B6" s="194" t="s">
+      <c r="B6" s="204" t="s">
         <v>141</v>
       </c>
       <c r="C6" s="118" t="s">
@@ -12741,7 +12779,7 @@
     </row>
     <row r="7" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
-      <c r="B7" s="190"/>
+      <c r="B7" s="200"/>
       <c r="C7" s="124" t="s">
         <v>142</v>
       </c>
@@ -12763,20 +12801,20 @@
       <c r="A8" s="7"/>
       <c r="B8" s="117"/>
       <c r="C8" s="97"/>
-      <c r="D8" s="169" t="s">
+      <c r="D8" s="176" t="s">
         <v>95</v>
       </c>
-      <c r="E8" s="169"/>
-      <c r="F8" s="169"/>
-      <c r="G8" s="169"/>
+      <c r="E8" s="176"/>
+      <c r="F8" s="176"/>
+      <c r="G8" s="176"/>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
-      <c r="B9" s="169" t="s">
+      <c r="B9" s="176" t="s">
         <v>140</v>
       </c>
-      <c r="C9" s="169"/>
+      <c r="C9" s="176"/>
       <c r="D9" s="139">
         <v>0.02</v>
       </c>
@@ -12793,7 +12831,7 @@
     </row>
     <row r="10" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
-      <c r="B10" s="194" t="s">
+      <c r="B10" s="204" t="s">
         <v>141</v>
       </c>
       <c r="C10" s="118" t="s">
@@ -12815,7 +12853,7 @@
     </row>
     <row r="11" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
-      <c r="B11" s="195"/>
+      <c r="B11" s="205"/>
       <c r="C11" s="121" t="s">
         <v>142</v>
       </c>
@@ -12835,10 +12873,10 @@
     </row>
     <row r="12" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
-      <c r="B12" s="191" t="s">
+      <c r="B12" s="201" t="s">
         <v>143</v>
       </c>
-      <c r="C12" s="192"/>
+      <c r="C12" s="202"/>
       <c r="D12" s="129">
         <v>0</v>
       </c>

</xml_diff>